<commit_message>
Branch:INV002 -> Deploy code this is live.
</commit_message>
<xml_diff>
--- a/App1.1/static/domestic_sort_file.xlsx
+++ b/App1.1/static/domestic_sort_file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6664" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6721" uniqueCount="398">
   <si>
     <t>main</t>
   </si>
@@ -1161,13 +1161,70 @@
   </si>
   <si>
     <t>NUT PULLER PLASTIC BAG</t>
+  </si>
+  <si>
+    <t>CONTROLLER BOX - 6 PIPE ( COMMON )  1 BAG X 200</t>
+  </si>
+  <si>
+    <t>6X10 SCREW NUT</t>
+  </si>
+  <si>
+    <t>6X10 SCREW TURBO CONTROLLER</t>
+  </si>
+  <si>
+    <t>4X13 SCREW TURBO CONTROLLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5X9 PAN PHILLIPS SCREW 3/8 &amp; 6/8 </t>
+  </si>
+  <si>
+    <t>REED SCREW 9.5</t>
+  </si>
+  <si>
+    <t>6.65 PIANO PATTI SCREW</t>
+  </si>
+  <si>
+    <t>7.13 PIANO COVER SCREW PAN PHILLIPS</t>
+  </si>
+  <si>
+    <t>16 TONES LABALE</t>
+  </si>
+  <si>
+    <t>18 TONES LABALE</t>
+  </si>
+  <si>
+    <t>20 TONES LABALE</t>
+  </si>
+  <si>
+    <t>22 TONES LABALE</t>
+  </si>
+  <si>
+    <t>30 TONES LABALE</t>
+  </si>
+  <si>
+    <t>31 TONES LABALE</t>
+  </si>
+  <si>
+    <t>32 TONES LABALE</t>
+  </si>
+  <si>
+    <t>BASURI SILVER STICKER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63 MM PIPE </t>
+  </si>
+  <si>
+    <t>65 MM PIPE</t>
+  </si>
+  <si>
+    <t>PIC16F72-ISP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1205,8 +1262,134 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1224,8 +1407,182 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1248,12 +1605,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1265,10 +1769,54 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="1" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
@@ -1860,11 +2408,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G1347"/>
+  <dimension ref="A1:G1366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4:F40"/>
+      <pane ySplit="1" topLeftCell="A1038" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1054" sqref="K1054"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -28382,6 +28930,216 @@
       </c>
       <c r="G1347" s="10" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="1348" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1348" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1348" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1348" s="4"/>
+      <c r="G1348" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1349" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1349" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1349" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1349" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1350" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1350" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D1350" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1350" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1351" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1351" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1351" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1351" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1352" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1352" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="D1352" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1352" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1353" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1353" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="D1353" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1353" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1354" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1354" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="D1354" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1354" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1355" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1355" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1355" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1355" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1356" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1356" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1356" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1356" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1357" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1357" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1357" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1357" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1358" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1358" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1358" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1358" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1359" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1359" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1359" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1359" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1360" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1360" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1360" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1360" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1361" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1361" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1361" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1361" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1362" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1362" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="D1362" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1362" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1363" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1363" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="D1363" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1363" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1364" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1364" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="D1364" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1364" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1365" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1365" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1365" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1365" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1366" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1366" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="D1366" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1366" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>